<commit_message>
Fixes on DataFill regarding multi-sheet processing. Stocks example working, without the styling. Style copying issues being chased.
</commit_message>
<xml_diff>
--- a/examples/stock-template.xlsx
+++ b/examples/stock-template.xlsx
@@ -20,13 +20,13 @@
     <t>{{ | 1 * years: | }}</t>
   </si>
   <si>
-    <t>{{ | companies | name }}</t>
+    <t>{{ | companies | name | | fill=:rowFormat }}</t>
   </si>
   <si>
-    <t>{{ A2 | 1 * years | value | fill:catFormat }}</t>
+    <t>{{ A2 | 1 * years | value | | fill=:rowFormat }}</t>
   </si>
   <si>
-    <t>{{ | companies * years | value | fill:catFormat }}</t>
+    <t>{{ | companies * years | value | | fill=:rowFormat }}</t>
   </si>
 </sst>
 </file>
@@ -70,7 +70,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -80,6 +80,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="11"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -123,13 +129,13 @@
     <xf numFmtId="49" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -152,8 +158,9 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffa7a7a7"/>
+      <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
 </styleSheet>

</xml_diff>

<commit_message>
Final fixes on XlsxPopulate styling patches.
</commit_message>
<xml_diff>
--- a/examples/stock-template.xlsx
+++ b/examples/stock-template.xlsx
@@ -20,13 +20,13 @@
     <t>{{ | 1 * years: | }}</t>
   </si>
   <si>
-    <t>{{ | companies | name | | fill=:rowFormat }}</t>
+    <t>{{ | companies | name | | :rowFormat }}</t>
   </si>
   <si>
-    <t>{{ A2 | 1 * years | value | | fill=:rowFormat }}</t>
+    <t>{{ A2 | 1 * years | value | }}</t>
   </si>
   <si>
-    <t>{{ | companies * years | value | | fill=:rowFormat }}</t>
+    <t>{{ | companies * years | value | }}</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Fixed a bug in default values extraction inside iteration. Disabled styling in stocks test - it is too slow and memory consuming.
</commit_message>
<xml_diff>
--- a/examples/stock-template.xlsx
+++ b/examples/stock-template.xlsx
@@ -23,10 +23,10 @@
     <t>{{ | companies | name | | :rowFormat }}</t>
   </si>
   <si>
-    <t>{{ A2 | 1 * years | value | }}</t>
+    <t>{{ A2 | 1 * years:$ | value | }}</t>
   </si>
   <si>
-    <t>{{ | companies * years | value | }}</t>
+    <t>{{ | companies * years:$ | value | }}</t>
   </si>
 </sst>
 </file>
@@ -1230,7 +1230,7 @@
   <cols>
     <col min="1" max="1" width="18.5" style="1" customWidth="1"/>
     <col min="2" max="11" width="11.5" style="1" customWidth="1"/>
-    <col min="12" max="256" width="11.8516" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="11.8516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.65" customHeight="1">
@@ -2574,7 +2574,7 @@
   <cols>
     <col min="1" max="1" width="18.5" style="6" customWidth="1"/>
     <col min="2" max="11" width="11.5" style="6" customWidth="1"/>
-    <col min="12" max="256" width="11.8516" style="6" customWidth="1"/>
+    <col min="12" max="16384" width="11.8516" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.65" customHeight="1">

</xml_diff>